<commit_message>
Added error vector to MLP
</commit_message>
<xml_diff>
--- a/Results/GA Parameters.xlsx
+++ b/Results/GA Parameters.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\white\Google Drive\School\CSCI-447 Machine Learning\P3 Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\white\OneDrive\School\CSCI-447 Machine Learning\Project3\CSCI447_P3\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,50 +23,103 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Bradley White</author>
+  </authors>
+  <commentList>
+    <comment ref="F6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Bradley White:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Integer stopped changing at 4200 generations</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>10 min</t>
-  </si>
-  <si>
-    <t>72 min</t>
-  </si>
-  <si>
-    <t>21 min</t>
-  </si>
-  <si>
-    <t>100/100/10000</t>
-  </si>
-  <si>
-    <t>5 hours</t>
-  </si>
-  <si>
-    <t>10/100/2000</t>
-  </si>
-  <si>
-    <t>100/100/2000</t>
-  </si>
-  <si>
-    <t>10/200/2000</t>
-  </si>
-  <si>
-    <t>Stopped changing around 9000 generations</t>
-  </si>
-  <si>
-    <t>Integer stopped changing around 4200 generations</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="12">
+  <si>
+    <t>ES</t>
+  </si>
+  <si>
+    <t>Generation</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>Converged</t>
+  </si>
+  <si>
+    <t>Children</t>
+  </si>
+  <si>
+    <t>Time(m)</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Population</t>
+  </si>
+  <si>
+    <t>GA</t>
+  </si>
+  <si>
+    <t>HL</t>
+  </si>
+  <si>
+    <t>HN</t>
+  </si>
+  <si>
+    <t>9000(4200)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -89,9 +142,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,71 +466,277 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="1" max="6" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>100</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2000</v>
+      </c>
+      <c r="E3" s="1">
+        <v>10</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="3">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>100</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D4" s="1">
+        <v>7746.3220000000001</v>
+      </c>
+      <c r="E4" s="1">
+        <v>72</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>200</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2000</v>
+      </c>
+      <c r="E5" s="1">
+        <v>21</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>100</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="1">
+        <v>10000</v>
+      </c>
+      <c r="D6" s="1">
+        <v>7508.2146409999996</v>
+      </c>
+      <c r="E6" s="1">
+        <v>300</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>100</v>
+      </c>
+      <c r="B11" s="1">
+        <v>250</v>
+      </c>
+      <c r="C11" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D11" s="1">
+        <v>6831.9115000000002</v>
+      </c>
+      <c r="E11" s="1">
+        <v>48</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>7746.3222380949501</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5">
-        <v>7508.2146413580404</v>
-      </c>
-      <c r="E5">
-        <f>C2/C5</f>
-        <v>1.0317129448358235</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>9</v>
+      <c r="G11" s="1">
+        <v>1</v>
+      </c>
+      <c r="H11" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>100</v>
+      </c>
+      <c r="B12" s="1">
+        <v>200</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D12" s="1">
+        <v>7060.3950000000004</v>
+      </c>
+      <c r="E12" s="1">
+        <v>43</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1</v>
+      </c>
+      <c r="H12" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>100</v>
+      </c>
+      <c r="B13" s="1">
+        <v>150</v>
+      </c>
+      <c r="C13" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D13" s="1">
+        <v>6654.1072000000004</v>
+      </c>
+      <c r="E13" s="1">
+        <v>37</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="1">
+        <v>1</v>
+      </c>
+      <c r="H13" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>100</v>
+      </c>
+      <c r="B14" s="1">
+        <v>100</v>
+      </c>
+      <c r="C14" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D14" s="1">
+        <v>6864.6840000000002</v>
+      </c>
+      <c r="E14" s="1">
+        <v>30</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1</v>
+      </c>
+      <c r="H14" s="1">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>